<commit_message>
mobile prediction file added
</commit_message>
<xml_diff>
--- a/devops.xlsx
+++ b/devops.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -324,7 +324,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,6 +334,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -373,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -382,7 +388,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -686,13 +698,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A102"/>
+  <dimension ref="A1:A104"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="23.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="23.433571428571426" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1075,133 +1087,143 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
       <c r="A77" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5">
       <c r="A78" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5">
       <c r="A79" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5">
       <c r="A80" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5">
       <c r="A81" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5">
       <c r="A82" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5">
       <c r="A83" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5">
       <c r="A84" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
       <c r="A85" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
       <c r="A86" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
       <c r="A87" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
       <c r="A88" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5">
       <c r="A89" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5">
       <c r="A90" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5">
       <c r="A91" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5">
       <c r="A92" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5">
       <c r="A93" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="19.5">
       <c r="A94" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="19.5">
       <c r="A95" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="19.5">
       <c r="A96" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
-      <c r="A97" s="2" t="s">
+      <c r="A97" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="19.5">
+      <c r="A98" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
-      <c r="A98" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="19.5">
+      <c r="A99" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
-      <c r="A99" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="19.5">
+      <c r="A100" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
-      <c r="A100" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="19.5">
+      <c r="A101" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
-      <c r="A101" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="19.5">
+      <c r="A102" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
-      <c r="A102" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
+      <c r="A103" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="19.5">
+      <c r="A104" s="2" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>